<commit_message>
function defined to scrape listed id and url made scripts pulls data in german format successful
</commit_message>
<xml_diff>
--- a/YourMOney_refdata.xlsx
+++ b/YourMOney_refdata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -634,7 +634,316 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>3.682192%</t>
+          <t>3.736986%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Schweizerische Eidgenossenschaft</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0.5 EIDG 30</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>27.05.2015</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>27.05.2030</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>315.377 Mio</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>103.00</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Nominal</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1'000</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>CHF</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>CH0224397171</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>22439717</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>0.50%</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+1 Jahr                                    </t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>26.05.</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>30/360</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>0.338889%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pfandbriefbank Schweizerischer Hypothekarinstitute AG</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.125 PB 23 S576</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>16.11.2012</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>16.11.2023</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>130 Mio</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>101.146</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Nominal</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>5'000</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>CHF</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>CH0199589588</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>19958958</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>1.125%</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+1 Jahr                                    </t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>15.11.</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>30/360</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>0.234375%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Pfandbriefzentrale der schweizerischen Kantonalbanken AG</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1 PZ 23 S427</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>13.11.2012</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>13.02.2023</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>295 Mio</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>100.934</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nominal</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>5'000</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>CHF</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>CH0198800325</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>19880032</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>1.00%</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+1 Jahr                                    </t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>12.02.</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>30/360</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>0.966667%</t>
         </is>
       </c>
     </row>

</xml_diff>